<commit_message>
add function to generate PO
</commit_message>
<xml_diff>
--- a/backend/static/PO TemplateLT.xlsx
+++ b/backend/static/PO TemplateLT.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10917"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dongxiaomu/Desktop/iMIS/backend/static/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA4D89D4-A759-C549-B4E4-FA4F779837BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="780" windowWidth="18720" windowHeight="11385"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,12 +20,17 @@
   <definedNames>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">Sheet1!$1:$16</definedName>
   </definedNames>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -237,6 +248,7 @@
         <b/>
         <sz val="10"/>
         <rFont val="宋体"/>
+        <charset val="134"/>
       </rPr>
       <t>海运发至</t>
     </r>
@@ -328,15 +340,14 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="5">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="4">
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
-    <numFmt numFmtId="165" formatCode="mm/dd/yy"/>
     <numFmt numFmtId="166" formatCode="dd\-mmm\-yy"/>
     <numFmt numFmtId="167" formatCode="[$-409]d\-mmm\-yy;@"/>
     <numFmt numFmtId="168" formatCode="&quot;$&quot;#,##0.0000"/>
   </numFmts>
-  <fonts count="30">
+  <fonts count="25">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -410,6 +421,7 @@
     <font>
       <sz val="9"/>
       <name val="宋体"/>
+      <charset val="134"/>
     </font>
     <font>
       <sz val="12"/>
@@ -449,15 +461,18 @@
       <b/>
       <sz val="10"/>
       <name val="宋体"/>
+      <charset val="134"/>
     </font>
     <font>
       <b/>
       <sz val="14"/>
       <name val="宋体"/>
+      <charset val="134"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="宋体"/>
+      <charset val="134"/>
     </font>
     <font>
       <b/>
@@ -477,33 +492,6 @@
       <name val="Arial Narrow"/>
       <family val="2"/>
     </font>
-    <font>
-      <sz val="10"/>
-      <name val="Gulim"/>
-      <family val="2"/>
-      <charset val="129"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Gulim"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="10"/>
-      <name val="Gulim"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <name val="Gulim"/>
-      <family val="2"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -513,7 +501,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="44">
+  <borders count="35">
     <border>
       <left/>
       <right/>
@@ -783,7 +771,62 @@
     </border>
     <border>
       <left/>
-      <right style="thin">
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="double">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
         <color indexed="64"/>
       </right>
       <top/>
@@ -791,114 +834,7 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="double">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
+      <left style="double">
         <color indexed="64"/>
       </left>
       <right/>
@@ -909,63 +845,12 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right style="medium">
         <color indexed="64"/>
       </right>
       <top/>
       <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -998,7 +883,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="180">
+  <cellXfs count="134">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1130,15 +1015,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1207,81 +1083,14 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="26" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="26" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="26" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="26" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="3" fontId="26" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="26" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="26" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="26" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="26" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="27" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="26" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="26" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="26" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="27" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="29" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="29" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1290,20 +1099,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="26" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="26" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="26" fillId="0" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" shrinkToFit="1"/>
@@ -1323,13 +1123,10 @@
     <xf numFmtId="0" fontId="22" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1338,50 +1135,66 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="26" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="26" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="26" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="167" fontId="9" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="24" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
@@ -1389,81 +1202,23 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="167" fontId="9" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="167" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="164" fontId="18" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="24" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment shrinkToFit="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment shrinkToFit="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="21" fillId="0" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="21" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="21" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1556,13 +1311,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>186690</xdr:colOff>
-      <xdr:row>26</xdr:row>
+      <xdr:row>25</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>167690</xdr:colOff>
-      <xdr:row>27</xdr:row>
+      <xdr:row>26</xdr:row>
       <xdr:rowOff>68580</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1570,7 +1325,7 @@
         <xdr:cNvPr id="1026" name="Text Box 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002040000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002040000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1965,41 +1720,38 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:V26"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="B1:S25"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="80" workbookViewId="0">
-      <selection activeCell="O12" sqref="O12"/>
+      <selection activeCell="H30" sqref="H30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="13"/>
   <cols>
-    <col min="1" max="1" width="1.28515625" style="21" customWidth="1"/>
-    <col min="2" max="2" width="5.5703125" style="19" customWidth="1"/>
-    <col min="3" max="3" width="7.140625" style="19" customWidth="1"/>
-    <col min="4" max="4" width="5.7109375" style="19" customWidth="1"/>
-    <col min="5" max="5" width="10.7109375" style="19" customWidth="1"/>
-    <col min="6" max="6" width="10.7109375" style="20" customWidth="1"/>
-    <col min="7" max="7" width="8.5703125" style="20" customWidth="1"/>
+    <col min="1" max="1" width="1.33203125" style="21" customWidth="1"/>
+    <col min="2" max="2" width="5.5" style="19" customWidth="1"/>
+    <col min="3" max="3" width="7.1640625" style="19" customWidth="1"/>
+    <col min="4" max="4" width="5.6640625" style="19" customWidth="1"/>
+    <col min="5" max="5" width="10.6640625" style="19" customWidth="1"/>
+    <col min="6" max="6" width="10.6640625" style="20" customWidth="1"/>
+    <col min="7" max="7" width="8.5" style="20" customWidth="1"/>
     <col min="8" max="8" width="14" style="20" customWidth="1"/>
-    <col min="9" max="9" width="3.85546875" style="20" hidden="1" customWidth="1"/>
-    <col min="10" max="10" width="2.28515625" style="20" hidden="1" customWidth="1"/>
-    <col min="11" max="11" width="10.85546875" style="20" customWidth="1"/>
-    <col min="12" max="12" width="26.7109375" style="22" customWidth="1"/>
-    <col min="13" max="13" width="11.7109375" style="1" hidden="1" customWidth="1"/>
-    <col min="14" max="14" width="12.5703125" style="127" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="10.42578125" style="2" customWidth="1"/>
-    <col min="16" max="16" width="15" style="4" customWidth="1"/>
-    <col min="17" max="17" width="16.28515625" style="4" customWidth="1"/>
-    <col min="18" max="18" width="13.42578125" style="4" customWidth="1"/>
-    <col min="19" max="19" width="12.85546875" style="29" customWidth="1"/>
-    <col min="20" max="20" width="13" style="29" customWidth="1"/>
-    <col min="21" max="21" width="15" style="29" customWidth="1"/>
-    <col min="22" max="22" width="16.28515625" style="29" customWidth="1"/>
-    <col min="23" max="16384" width="9.140625" style="21"/>
+    <col min="9" max="9" width="10.83203125" style="20" customWidth="1"/>
+    <col min="10" max="10" width="26.6640625" style="22" customWidth="1"/>
+    <col min="11" max="11" width="12.5" style="96" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.5" style="2" customWidth="1"/>
+    <col min="13" max="13" width="15" style="4" customWidth="1"/>
+    <col min="14" max="14" width="16.33203125" style="4" customWidth="1"/>
+    <col min="15" max="15" width="13.5" style="4" customWidth="1"/>
+    <col min="16" max="16" width="12.83203125" style="29" customWidth="1"/>
+    <col min="17" max="17" width="13" style="29" customWidth="1"/>
+    <col min="18" max="18" width="15" style="29" customWidth="1"/>
+    <col min="19" max="19" width="16.33203125" style="29" customWidth="1"/>
+    <col min="20" max="16384" width="9.1640625" style="21"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:22" ht="35.25">
+    <row r="1" spans="2:19" ht="35">
       <c r="B1" s="3" t="s">
         <v>13</v>
       </c>
@@ -2008,24 +1760,21 @@
       <c r="H1" s="11"/>
       <c r="I1" s="11"/>
       <c r="J1" s="11"/>
-      <c r="K1" s="11"/>
-      <c r="L1" s="11"/>
-      <c r="M1" s="37"/>
-      <c r="N1" s="126" t="s">
+      <c r="K1" s="95" t="s">
         <v>17</v>
       </c>
-      <c r="O1" s="37"/>
-      <c r="P1" s="38" t="s">
+      <c r="L1" s="37"/>
+      <c r="M1" s="38" t="s">
         <v>18</v>
       </c>
-      <c r="Q1" s="12"/>
-      <c r="R1" s="12"/>
-      <c r="S1" s="28"/>
-      <c r="T1" s="12" t="s">
+      <c r="N1" s="12"/>
+      <c r="O1" s="12"/>
+      <c r="P1" s="28"/>
+      <c r="Q1" s="12" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="2:22" s="2" customFormat="1" ht="15.95" customHeight="1">
+    <row r="2" spans="2:19" s="2" customFormat="1" ht="16" customHeight="1">
       <c r="B2" s="19" t="s">
         <v>64</v>
       </c>
@@ -2036,22 +1785,19 @@
       <c r="G2" s="20"/>
       <c r="H2" s="20"/>
       <c r="I2" s="20"/>
-      <c r="J2" s="20"/>
-      <c r="K2" s="20"/>
-      <c r="L2" s="22"/>
-      <c r="M2" s="1"/>
-      <c r="N2" s="127"/>
-      <c r="P2" s="4"/>
-      <c r="Q2" s="5"/>
-      <c r="R2" s="5"/>
-      <c r="S2" s="165" t="s">
+      <c r="J2" s="22"/>
+      <c r="K2" s="96"/>
+      <c r="M2" s="4"/>
+      <c r="N2" s="5"/>
+      <c r="O2" s="5"/>
+      <c r="P2" s="121" t="s">
         <v>38</v>
       </c>
-      <c r="T2" s="165"/>
-      <c r="U2" s="168"/>
-      <c r="V2" s="169"/>
+      <c r="Q2" s="121"/>
+      <c r="R2" s="124"/>
+      <c r="S2" s="125"/>
     </row>
-    <row r="3" spans="2:22" s="2" customFormat="1" ht="15.95" customHeight="1">
+    <row r="3" spans="2:19" s="2" customFormat="1" ht="16" customHeight="1">
       <c r="B3" s="19" t="s">
         <v>65</v>
       </c>
@@ -2062,23 +1808,20 @@
       <c r="G3" s="23"/>
       <c r="H3" s="23"/>
       <c r="I3" s="23"/>
-      <c r="J3" s="23"/>
-      <c r="K3" s="23"/>
-      <c r="L3" s="21"/>
-      <c r="M3" s="19"/>
-      <c r="N3" s="128"/>
-      <c r="O3" s="22"/>
-      <c r="P3" s="1"/>
-      <c r="Q3" s="6"/>
-      <c r="R3" s="6"/>
-      <c r="S3" s="165" t="s">
+      <c r="J3" s="21"/>
+      <c r="K3" s="97"/>
+      <c r="L3" s="22"/>
+      <c r="M3" s="1"/>
+      <c r="N3" s="6"/>
+      <c r="O3" s="6"/>
+      <c r="P3" s="121" t="s">
         <v>37</v>
       </c>
-      <c r="T3" s="165"/>
-      <c r="U3" s="168"/>
-      <c r="V3" s="169"/>
+      <c r="Q3" s="121"/>
+      <c r="R3" s="124"/>
+      <c r="S3" s="125"/>
     </row>
-    <row r="4" spans="2:22" s="2" customFormat="1" ht="12.75" customHeight="1">
+    <row r="4" spans="2:19" s="2" customFormat="1" ht="12.75" customHeight="1">
       <c r="B4" s="19" t="s">
         <v>61</v>
       </c>
@@ -2089,23 +1832,20 @@
       <c r="G4" s="23"/>
       <c r="H4" s="23"/>
       <c r="I4" s="23"/>
-      <c r="J4" s="23"/>
-      <c r="K4" s="23"/>
-      <c r="L4" s="21"/>
-      <c r="M4" s="19"/>
-      <c r="N4" s="128"/>
-      <c r="O4" s="22"/>
-      <c r="P4" s="1"/>
-      <c r="Q4" s="1"/>
-      <c r="R4" s="1"/>
-      <c r="S4" s="166" t="s">
+      <c r="J4" s="21"/>
+      <c r="K4" s="97"/>
+      <c r="L4" s="22"/>
+      <c r="M4" s="1"/>
+      <c r="N4" s="1"/>
+      <c r="O4" s="1"/>
+      <c r="P4" s="122" t="s">
         <v>46</v>
       </c>
-      <c r="T4" s="166"/>
-      <c r="U4" s="166"/>
-      <c r="V4" s="166"/>
+      <c r="Q4" s="122"/>
+      <c r="R4" s="122"/>
+      <c r="S4" s="122"/>
     </row>
-    <row r="5" spans="2:22" s="2" customFormat="1">
+    <row r="5" spans="2:19" s="2" customFormat="1">
       <c r="B5" s="4"/>
       <c r="C5" s="4"/>
       <c r="D5" s="4"/>
@@ -2114,21 +1854,18 @@
       <c r="G5" s="24"/>
       <c r="H5" s="24"/>
       <c r="I5" s="24"/>
-      <c r="J5" s="24"/>
-      <c r="K5" s="24"/>
-      <c r="L5" s="21"/>
-      <c r="M5" s="19"/>
-      <c r="N5" s="128"/>
-      <c r="O5" s="22"/>
-      <c r="P5" s="1"/>
-      <c r="Q5" s="1"/>
-      <c r="R5" s="1"/>
-      <c r="S5" s="166"/>
-      <c r="T5" s="166"/>
-      <c r="U5" s="166"/>
-      <c r="V5" s="166"/>
+      <c r="J5" s="21"/>
+      <c r="K5" s="97"/>
+      <c r="L5" s="22"/>
+      <c r="M5" s="1"/>
+      <c r="N5" s="1"/>
+      <c r="O5" s="1"/>
+      <c r="P5" s="122"/>
+      <c r="Q5" s="122"/>
+      <c r="R5" s="122"/>
+      <c r="S5" s="122"/>
     </row>
-    <row r="6" spans="2:22" s="2" customFormat="1" ht="12.75" customHeight="1">
+    <row r="6" spans="2:19" s="2" customFormat="1" ht="12.75" customHeight="1">
       <c r="B6" s="19"/>
       <c r="C6" s="4"/>
       <c r="D6" s="4"/>
@@ -2137,23 +1874,20 @@
       <c r="G6" s="24"/>
       <c r="H6" s="24"/>
       <c r="I6" s="24"/>
-      <c r="J6" s="24"/>
-      <c r="K6" s="24"/>
-      <c r="L6" s="21"/>
-      <c r="M6" s="19"/>
-      <c r="N6" s="128"/>
-      <c r="O6" s="22"/>
-      <c r="P6" s="1"/>
-      <c r="Q6" s="1"/>
-      <c r="R6" s="1"/>
-      <c r="S6" s="167" t="s">
+      <c r="J6" s="21"/>
+      <c r="K6" s="97"/>
+      <c r="L6" s="22"/>
+      <c r="M6" s="1"/>
+      <c r="N6" s="1"/>
+      <c r="O6" s="1"/>
+      <c r="P6" s="123" t="s">
         <v>20</v>
       </c>
-      <c r="T6" s="167"/>
-      <c r="U6" s="167"/>
-      <c r="V6" s="167"/>
+      <c r="Q6" s="123"/>
+      <c r="R6" s="123"/>
+      <c r="S6" s="123"/>
     </row>
-    <row r="7" spans="2:22" s="2" customFormat="1" ht="18" customHeight="1" thickBot="1">
+    <row r="7" spans="2:19" s="2" customFormat="1" ht="18" customHeight="1" thickBot="1">
       <c r="B7" s="4"/>
       <c r="C7" s="4"/>
       <c r="D7" s="4"/>
@@ -2162,22 +1896,19 @@
       <c r="G7" s="24"/>
       <c r="H7" s="24"/>
       <c r="I7" s="24"/>
-      <c r="J7" s="24"/>
-      <c r="K7" s="24"/>
-      <c r="L7" s="21"/>
-      <c r="M7" s="19"/>
-      <c r="N7" s="128"/>
-      <c r="O7" s="22"/>
-      <c r="P7" s="1"/>
-      <c r="Q7" s="1"/>
-      <c r="R7" s="1"/>
-      <c r="S7" s="167"/>
-      <c r="T7" s="167"/>
-      <c r="U7" s="167"/>
-      <c r="V7" s="167"/>
+      <c r="J7" s="21"/>
+      <c r="K7" s="97"/>
+      <c r="L7" s="22"/>
+      <c r="M7" s="1"/>
+      <c r="N7" s="1"/>
+      <c r="O7" s="1"/>
+      <c r="P7" s="123"/>
+      <c r="Q7" s="123"/>
+      <c r="R7" s="123"/>
+      <c r="S7" s="123"/>
     </row>
-    <row r="8" spans="2:22" s="22" customFormat="1" ht="15.95" customHeight="1">
-      <c r="B8" s="70" t="s">
+    <row r="8" spans="2:19" s="22" customFormat="1" ht="16" customHeight="1">
+      <c r="B8" s="67" t="s">
         <v>39</v>
       </c>
       <c r="C8" s="58"/>
@@ -2186,26 +1917,23 @@
       <c r="F8" s="58"/>
       <c r="G8" s="58"/>
       <c r="H8" s="58"/>
-      <c r="I8" s="58"/>
-      <c r="J8" s="58"/>
-      <c r="K8" s="141"/>
-      <c r="L8" s="44"/>
-      <c r="M8" s="62"/>
-      <c r="N8" s="129"/>
-      <c r="O8" s="119" t="s">
+      <c r="I8" s="106"/>
+      <c r="J8" s="44"/>
+      <c r="K8" s="98"/>
+      <c r="L8" s="91" t="s">
         <v>47</v>
       </c>
-      <c r="P8" s="120"/>
-      <c r="Q8" s="120"/>
-      <c r="R8" s="121"/>
-      <c r="S8" s="137" t="s">
+      <c r="M8" s="92"/>
+      <c r="N8" s="92"/>
+      <c r="O8" s="93"/>
+      <c r="P8" s="105" t="s">
         <v>48</v>
       </c>
-      <c r="T8" s="120"/>
-      <c r="U8" s="120"/>
-      <c r="V8" s="122"/>
+      <c r="Q8" s="92"/>
+      <c r="R8" s="92"/>
+      <c r="S8" s="94"/>
     </row>
-    <row r="9" spans="2:22" s="25" customFormat="1" ht="15.95" customHeight="1">
+    <row r="9" spans="2:19" s="25" customFormat="1" ht="16" customHeight="1">
       <c r="B9" s="59"/>
       <c r="C9" s="60"/>
       <c r="D9" s="60"/>
@@ -2213,74 +1941,65 @@
       <c r="F9" s="60"/>
       <c r="G9" s="60"/>
       <c r="H9" s="60"/>
-      <c r="I9" s="60"/>
-      <c r="J9" s="60"/>
-      <c r="K9" s="142"/>
-      <c r="L9" s="55"/>
-      <c r="M9" s="63"/>
-      <c r="N9" s="130"/>
-      <c r="O9" s="46" t="s">
+      <c r="I9" s="107"/>
+      <c r="J9" s="55"/>
+      <c r="K9" s="99"/>
+      <c r="L9" s="46" t="s">
         <v>19</v>
       </c>
-      <c r="P9" s="47"/>
-      <c r="Q9" s="47"/>
-      <c r="R9" s="48"/>
-      <c r="S9" s="170"/>
-      <c r="T9" s="171"/>
-      <c r="U9" s="171"/>
-      <c r="V9" s="172"/>
+      <c r="M9" s="47"/>
+      <c r="N9" s="47"/>
+      <c r="O9" s="48"/>
+      <c r="P9" s="128"/>
+      <c r="Q9" s="129"/>
+      <c r="R9" s="129"/>
+      <c r="S9" s="130"/>
     </row>
-    <row r="10" spans="2:22" s="25" customFormat="1" ht="15.75">
+    <row r="10" spans="2:19" s="25" customFormat="1" ht="16">
       <c r="B10" s="54"/>
       <c r="C10" s="55"/>
       <c r="D10" s="55"/>
       <c r="E10" s="55"/>
       <c r="F10" s="55"/>
       <c r="G10" s="55"/>
-      <c r="H10" s="143"/>
-      <c r="I10" s="143"/>
-      <c r="J10" s="143"/>
-      <c r="K10" s="144"/>
-      <c r="L10" s="55"/>
-      <c r="M10" s="61"/>
-      <c r="N10" s="130"/>
-      <c r="O10" s="49" t="s">
+      <c r="H10" s="55"/>
+      <c r="I10" s="108"/>
+      <c r="J10" s="55"/>
+      <c r="K10" s="99"/>
+      <c r="L10" s="49" t="s">
         <v>66</v>
       </c>
-      <c r="P10"/>
-      <c r="Q10"/>
-      <c r="R10" s="50"/>
-      <c r="S10" s="170"/>
-      <c r="T10" s="171"/>
-      <c r="U10" s="171"/>
-      <c r="V10" s="172"/>
+      <c r="M10"/>
+      <c r="N10"/>
+      <c r="O10" s="50"/>
+      <c r="P10" s="128"/>
+      <c r="Q10" s="129"/>
+      <c r="R10" s="129"/>
+      <c r="S10" s="130"/>
     </row>
-    <row r="11" spans="2:22" s="25" customFormat="1" ht="15.75">
+    <row r="11" spans="2:19" s="25" customFormat="1" ht="16">
       <c r="B11" s="54"/>
       <c r="C11" s="55"/>
       <c r="D11" s="55"/>
       <c r="E11" s="55"/>
       <c r="F11" s="55"/>
       <c r="G11" s="55"/>
-      <c r="H11" s="143"/>
-      <c r="I11" s="143"/>
-      <c r="J11" s="143"/>
-      <c r="K11" s="144"/>
-      <c r="L11" s="55"/>
-      <c r="M11" s="61"/>
-      <c r="N11" s="130"/>
-      <c r="O11" s="49" t="s">
+      <c r="H11" s="55"/>
+      <c r="I11" s="108"/>
+      <c r="J11" s="55"/>
+      <c r="K11" s="99"/>
+      <c r="L11" s="49" t="s">
         <v>67</v>
       </c>
-      <c r="P11"/>
-      <c r="Q11"/>
-      <c r="R11" s="50"/>
-      <c r="S11" s="170"/>
-      <c r="T11" s="171"/>
-      <c r="U11" s="171"/>
-      <c r="V11" s="172"/>
+      <c r="M11"/>
+      <c r="N11"/>
+      <c r="O11" s="50"/>
+      <c r="P11" s="128"/>
+      <c r="Q11" s="129"/>
+      <c r="R11" s="129"/>
+      <c r="S11" s="130"/>
     </row>
-    <row r="12" spans="2:22" s="25" customFormat="1" ht="16.5" thickBot="1">
+    <row r="12" spans="2:19" s="25" customFormat="1" ht="17" thickBot="1">
       <c r="B12" s="56"/>
       <c r="C12" s="57"/>
       <c r="D12" s="57"/>
@@ -2288,379 +2007,335 @@
       <c r="F12" s="57"/>
       <c r="G12" s="57"/>
       <c r="H12" s="57"/>
-      <c r="I12" s="57"/>
-      <c r="J12" s="57"/>
-      <c r="K12" s="145"/>
-      <c r="L12" s="55"/>
-      <c r="M12" s="61"/>
-      <c r="N12" s="130"/>
-      <c r="O12" s="51" t="s">
+      <c r="I12" s="109"/>
+      <c r="J12" s="55"/>
+      <c r="K12" s="99"/>
+      <c r="L12" s="51" t="s">
         <v>62</v>
       </c>
-      <c r="P12" s="52"/>
-      <c r="Q12" s="52"/>
-      <c r="R12" s="53"/>
-      <c r="S12" s="173"/>
-      <c r="T12" s="174"/>
-      <c r="U12" s="174"/>
-      <c r="V12" s="175"/>
+      <c r="M12" s="52"/>
+      <c r="N12" s="52"/>
+      <c r="O12" s="53"/>
+      <c r="P12" s="131"/>
+      <c r="Q12" s="132"/>
+      <c r="R12" s="132"/>
+      <c r="S12" s="133"/>
     </row>
-    <row r="13" spans="2:22" ht="6.95" customHeight="1" thickBot="1">
+    <row r="13" spans="2:19" ht="7" customHeight="1" thickBot="1">
       <c r="C13" s="26"/>
     </row>
-    <row r="14" spans="2:22" s="77" customFormat="1" ht="22.5" customHeight="1">
-      <c r="B14" s="76" t="s">
+    <row r="14" spans="2:19" s="74" customFormat="1" ht="22.5" customHeight="1">
+      <c r="B14" s="73" t="s">
         <v>63</v>
       </c>
-      <c r="C14" s="73" t="s">
+      <c r="C14" s="70" t="s">
         <v>27</v>
       </c>
-      <c r="D14" s="73" t="s">
+      <c r="D14" s="70" t="s">
         <v>22</v>
       </c>
-      <c r="E14" s="73" t="s">
+      <c r="E14" s="70" t="s">
         <v>23</v>
       </c>
-      <c r="F14" s="73" t="s">
+      <c r="F14" s="70" t="s">
         <v>28</v>
       </c>
-      <c r="G14" s="73" t="s">
+      <c r="G14" s="70" t="s">
         <v>29</v>
       </c>
-      <c r="H14" s="73" t="s">
+      <c r="H14" s="70" t="s">
         <v>58</v>
       </c>
-      <c r="I14" s="73"/>
-      <c r="J14" s="73"/>
-      <c r="K14" s="74" t="s">
+      <c r="I14" s="71" t="s">
         <v>43</v>
       </c>
-      <c r="L14" s="146" t="s">
+      <c r="J14" s="71" t="s">
         <v>35</v>
       </c>
-      <c r="M14" s="147"/>
-      <c r="N14" s="131" t="s">
+      <c r="K14" s="100" t="s">
         <v>24</v>
       </c>
-      <c r="O14" s="73" t="s">
+      <c r="L14" s="70" t="s">
         <v>30</v>
       </c>
-      <c r="P14" s="73" t="s">
+      <c r="M14" s="70" t="s">
         <v>49</v>
       </c>
-      <c r="Q14" s="73" t="s">
+      <c r="N14" s="70" t="s">
         <v>25</v>
       </c>
-      <c r="R14" s="73" t="s">
+      <c r="O14" s="70" t="s">
         <v>26</v>
       </c>
-      <c r="S14" s="73" t="s">
+      <c r="P14" s="70" t="s">
         <v>31</v>
       </c>
-      <c r="T14" s="73" t="s">
+      <c r="Q14" s="70" t="s">
         <v>32</v>
       </c>
-      <c r="U14" s="73" t="s">
+      <c r="R14" s="70" t="s">
         <v>33</v>
       </c>
-      <c r="V14" s="75" t="s">
+      <c r="S14" s="72" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="15" spans="2:22" s="64" customFormat="1" ht="15.95" customHeight="1">
-      <c r="B15" s="78" t="s">
+    <row r="15" spans="2:19" s="61" customFormat="1" ht="16" customHeight="1">
+      <c r="B15" s="75" t="s">
         <v>4</v>
       </c>
-      <c r="C15" s="66" t="s">
+      <c r="C15" s="63" t="s">
         <v>0</v>
       </c>
-      <c r="D15" s="66" t="s">
+      <c r="D15" s="63" t="s">
         <v>1</v>
       </c>
-      <c r="E15" s="66" t="s">
+      <c r="E15" s="63" t="s">
         <v>8</v>
       </c>
-      <c r="F15" s="66" t="s">
+      <c r="F15" s="63" t="s">
         <v>9</v>
       </c>
-      <c r="G15" s="66" t="s">
+      <c r="G15" s="63" t="s">
         <v>3</v>
       </c>
-      <c r="H15" s="66" t="s">
+      <c r="H15" s="63" t="s">
         <v>59</v>
       </c>
-      <c r="I15" s="66"/>
-      <c r="J15" s="66"/>
-      <c r="K15" s="83" t="s">
+      <c r="I15" s="80" t="s">
         <v>44</v>
       </c>
-      <c r="L15" s="148" t="s">
+      <c r="J15" s="80" t="s">
         <v>40</v>
       </c>
-      <c r="M15" s="149"/>
-      <c r="N15" s="152" t="s">
+      <c r="K15" s="126" t="s">
         <v>41</v>
       </c>
-      <c r="O15" s="67" t="s">
+      <c r="L15" s="64" t="s">
         <v>21</v>
       </c>
-      <c r="P15" s="67" t="s">
+      <c r="M15" s="64" t="s">
         <v>15</v>
       </c>
-      <c r="Q15" s="67" t="s">
+      <c r="N15" s="64" t="s">
         <v>6</v>
       </c>
-      <c r="R15" s="67" t="s">
+      <c r="O15" s="64" t="s">
         <v>1</v>
       </c>
-      <c r="S15" s="71" t="s">
+      <c r="P15" s="68" t="s">
         <v>50</v>
       </c>
-      <c r="T15" s="71" t="s">
+      <c r="Q15" s="68" t="s">
         <v>1</v>
       </c>
-      <c r="U15" s="68" t="s">
+      <c r="R15" s="65" t="s">
         <v>52</v>
       </c>
-      <c r="V15" s="69" t="s">
+      <c r="S15" s="66" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="16" spans="2:22" s="64" customFormat="1" ht="15.95" customHeight="1">
-      <c r="B16" s="79"/>
-      <c r="C16" s="65"/>
-      <c r="D16" s="65"/>
+    <row r="16" spans="2:19" s="61" customFormat="1" ht="16" customHeight="1">
+      <c r="B16" s="76"/>
+      <c r="C16" s="62"/>
+      <c r="D16" s="62"/>
       <c r="E16" s="7" t="s">
         <v>10</v>
       </c>
       <c r="F16" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="G16" s="80"/>
-      <c r="H16" s="81" t="s">
+      <c r="G16" s="77"/>
+      <c r="H16" s="78" t="s">
         <v>60</v>
       </c>
-      <c r="I16" s="81"/>
+      <c r="I16" s="81" t="s">
+        <v>45</v>
+      </c>
       <c r="J16" s="81"/>
-      <c r="K16" s="84" t="s">
-        <v>45</v>
-      </c>
-      <c r="L16" s="150"/>
-      <c r="M16" s="151"/>
-      <c r="N16" s="153"/>
+      <c r="K16" s="127"/>
+      <c r="L16" s="27" t="s">
+        <v>12</v>
+      </c>
+      <c r="M16" s="27" t="s">
+        <v>14</v>
+      </c>
+      <c r="N16" s="27" t="s">
+        <v>14</v>
+      </c>
       <c r="O16" s="27" t="s">
-        <v>12</v>
-      </c>
-      <c r="P16" s="27" t="s">
-        <v>14</v>
-      </c>
-      <c r="Q16" s="27" t="s">
-        <v>14</v>
-      </c>
-      <c r="R16" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="S16" s="72" t="s">
+      <c r="P16" s="69" t="s">
         <v>51</v>
       </c>
-      <c r="T16" s="72" t="s">
+      <c r="Q16" s="69" t="s">
         <v>5</v>
       </c>
-      <c r="U16" s="45" t="s">
+      <c r="R16" s="45" t="s">
         <v>53</v>
       </c>
-      <c r="V16" s="30" t="s">
+      <c r="S16" s="30" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="1:22" s="94" customFormat="1" ht="45.95" customHeight="1">
-      <c r="A17" s="88"/>
-      <c r="B17" s="110"/>
-      <c r="C17" s="105"/>
-      <c r="D17" s="89"/>
-      <c r="E17" s="139"/>
-      <c r="F17" s="138"/>
-      <c r="G17" s="140"/>
-      <c r="H17" s="90"/>
-      <c r="I17" s="90"/>
-      <c r="J17" s="90"/>
-      <c r="K17" s="107"/>
-      <c r="L17" s="178"/>
-      <c r="M17" s="179"/>
-      <c r="N17" s="132"/>
-      <c r="O17" s="106"/>
-      <c r="P17" s="91"/>
-      <c r="Q17" s="91"/>
-      <c r="R17" s="89"/>
-      <c r="S17" s="92"/>
-      <c r="T17" s="93"/>
-      <c r="U17" s="108" t="str">
-        <f>IF(ROUND(R17*S17,2),ROUND(R17*S17,2),"")</f>
-        <v/>
-      </c>
-      <c r="V17" s="109" t="str">
-        <f>IF(C17*(T17+R17*S17),C17*(T17+R17*S17),"")</f>
-        <v/>
-      </c>
+    <row r="17" spans="2:19" ht="6" customHeight="1">
+      <c r="B17" s="13"/>
+      <c r="C17" s="14"/>
+      <c r="D17" s="9"/>
+      <c r="E17" s="15"/>
+      <c r="F17" s="15"/>
+      <c r="G17" s="8"/>
+      <c r="H17" s="8"/>
+      <c r="I17" s="8"/>
+      <c r="J17" s="10"/>
+      <c r="K17" s="101"/>
+      <c r="L17" s="9"/>
+      <c r="M17" s="16"/>
+      <c r="N17" s="16"/>
+      <c r="O17" s="31"/>
+      <c r="P17" s="32"/>
+      <c r="Q17" s="32"/>
+      <c r="R17" s="32"/>
+      <c r="S17" s="35"/>
     </row>
-    <row r="18" spans="1:22" s="94" customFormat="1" ht="45.95" customHeight="1" thickBot="1">
-      <c r="B18" s="111"/>
-      <c r="C18" s="95"/>
-      <c r="D18" s="96"/>
-      <c r="E18" s="123"/>
-      <c r="F18" s="124"/>
-      <c r="G18" s="97"/>
-      <c r="H18" s="125"/>
-      <c r="I18" s="98"/>
-      <c r="J18" s="98"/>
-      <c r="K18" s="99"/>
-      <c r="L18" s="176"/>
-      <c r="M18" s="177"/>
-      <c r="N18" s="99"/>
-      <c r="O18" s="100"/>
-      <c r="P18" s="101"/>
-      <c r="Q18" s="101"/>
-      <c r="R18" s="102"/>
-      <c r="S18" s="103"/>
-      <c r="T18" s="103"/>
-      <c r="U18" s="103" t="str">
-        <f>IF(ROUND(R18*S18,2),ROUND(R18*S18,2),"")</f>
-        <v/>
-      </c>
-      <c r="V18" s="104" t="str">
-        <f>IF(C18*(T18+R18*S18),C18*(T18+R18*S18),"")</f>
-        <v/>
-      </c>
+    <row r="18" spans="2:19" ht="6" customHeight="1">
+      <c r="B18" s="13"/>
+      <c r="C18" s="14"/>
+      <c r="D18" s="9"/>
+      <c r="E18" s="15"/>
+      <c r="F18" s="15"/>
+      <c r="G18" s="8"/>
+      <c r="H18" s="8"/>
+      <c r="I18" s="8"/>
+      <c r="J18" s="10"/>
+      <c r="K18" s="101"/>
+      <c r="L18" s="9"/>
+      <c r="M18" s="16"/>
+      <c r="N18" s="16"/>
+      <c r="O18" s="31"/>
+      <c r="P18" s="32"/>
+      <c r="Q18" s="32"/>
+      <c r="R18" s="32"/>
+      <c r="S18" s="35"/>
     </row>
-    <row r="19" spans="1:22" ht="6" customHeight="1">
-      <c r="B19" s="13"/>
-      <c r="C19" s="14"/>
-      <c r="D19" s="9"/>
-      <c r="E19" s="15"/>
-      <c r="F19" s="15"/>
-      <c r="G19" s="8"/>
-      <c r="H19" s="8"/>
-      <c r="I19" s="8"/>
-      <c r="J19" s="8"/>
-      <c r="K19" s="8"/>
-      <c r="L19" s="10"/>
-      <c r="M19" s="9"/>
-      <c r="N19" s="133"/>
-      <c r="O19" s="9"/>
-      <c r="P19" s="16"/>
-      <c r="Q19" s="16"/>
-      <c r="R19" s="31"/>
-      <c r="S19" s="32"/>
-      <c r="T19" s="32"/>
-      <c r="U19" s="32"/>
-      <c r="V19" s="35"/>
+    <row r="19" spans="2:19" ht="16" customHeight="1" thickBot="1">
+      <c r="M19" s="17"/>
+      <c r="N19" s="33"/>
+      <c r="O19" s="33"/>
+      <c r="P19" s="79" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q19" s="36" t="s">
+        <v>42</v>
+      </c>
+      <c r="R19" s="116" t="e">
+        <f>SUM(#REF!)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="S19" s="117"/>
     </row>
-    <row r="20" spans="1:22" ht="15.95" customHeight="1" thickBot="1">
-      <c r="P20" s="17"/>
-      <c r="Q20" s="33"/>
-      <c r="R20" s="33"/>
-      <c r="S20" s="82" t="s">
-        <v>36</v>
-      </c>
-      <c r="T20" s="36" t="s">
-        <v>42</v>
-      </c>
-      <c r="U20" s="163">
-        <f>SUM(V17:V18)</f>
-        <v>0</v>
-      </c>
-      <c r="V20" s="164"/>
+    <row r="20" spans="2:19" ht="16" customHeight="1" thickTop="1">
+      <c r="B20" s="85" t="s">
+        <v>57</v>
+      </c>
+      <c r="C20" s="86"/>
+      <c r="D20" s="86"/>
+      <c r="E20" s="86"/>
+      <c r="F20" s="87"/>
+      <c r="G20" s="87"/>
+      <c r="H20" s="87"/>
+      <c r="I20" s="87"/>
+      <c r="J20" s="88"/>
+      <c r="K20" s="102"/>
+      <c r="L20" s="89"/>
+      <c r="M20" s="90"/>
+      <c r="N20" s="33"/>
+      <c r="O20" s="33"/>
+      <c r="P20" s="34"/>
+      <c r="Q20" s="43"/>
+      <c r="R20" s="43"/>
+      <c r="S20" s="44"/>
     </row>
-    <row r="21" spans="1:22" ht="15.95" customHeight="1" thickTop="1">
-      <c r="B21" s="112" t="s">
-        <v>57</v>
-      </c>
-      <c r="C21" s="113"/>
-      <c r="D21" s="113"/>
-      <c r="E21" s="113"/>
-      <c r="F21" s="114"/>
-      <c r="G21" s="114"/>
-      <c r="H21" s="114"/>
-      <c r="I21" s="114"/>
-      <c r="J21" s="114"/>
-      <c r="K21" s="114"/>
-      <c r="L21" s="115"/>
-      <c r="M21" s="116"/>
-      <c r="N21" s="134"/>
-      <c r="O21" s="117"/>
-      <c r="P21" s="118"/>
-      <c r="Q21" s="33"/>
-      <c r="R21" s="33"/>
-      <c r="S21" s="34"/>
-      <c r="T21" s="43"/>
-      <c r="U21" s="43"/>
-      <c r="V21" s="44"/>
+    <row r="21" spans="2:19">
+      <c r="B21" s="110"/>
+      <c r="C21" s="111"/>
+      <c r="D21" s="111"/>
+      <c r="E21" s="111"/>
+      <c r="F21" s="111"/>
+      <c r="G21" s="111"/>
+      <c r="H21" s="111"/>
+      <c r="I21" s="111"/>
+      <c r="J21" s="111"/>
+      <c r="K21" s="111"/>
+      <c r="L21" s="111"/>
+      <c r="M21" s="112"/>
     </row>
-    <row r="22" spans="1:22">
-      <c r="B22" s="154"/>
-      <c r="C22" s="155"/>
-      <c r="D22" s="155"/>
-      <c r="E22" s="155"/>
-      <c r="F22" s="155"/>
-      <c r="G22" s="155"/>
-      <c r="H22" s="155"/>
-      <c r="I22" s="155"/>
-      <c r="J22" s="155"/>
-      <c r="K22" s="155"/>
-      <c r="L22" s="155"/>
-      <c r="M22" s="155"/>
-      <c r="N22" s="155"/>
-      <c r="O22" s="155"/>
-      <c r="P22" s="156"/>
+    <row r="22" spans="2:19" ht="14">
+      <c r="B22" s="110"/>
+      <c r="C22" s="111"/>
+      <c r="D22" s="111"/>
+      <c r="E22" s="111"/>
+      <c r="F22" s="111"/>
+      <c r="G22" s="111"/>
+      <c r="H22" s="111"/>
+      <c r="I22" s="111"/>
+      <c r="J22" s="111"/>
+      <c r="K22" s="111"/>
+      <c r="L22" s="111"/>
+      <c r="M22" s="112"/>
+      <c r="P22" s="83" t="s">
+        <v>54</v>
+      </c>
+      <c r="Q22" s="84"/>
+      <c r="R22" s="42" t="s">
+        <v>56</v>
+      </c>
     </row>
-    <row r="23" spans="1:22">
-      <c r="B23" s="154"/>
-      <c r="C23" s="155"/>
-      <c r="D23" s="155"/>
-      <c r="E23" s="155"/>
-      <c r="F23" s="155"/>
-      <c r="G23" s="155"/>
-      <c r="H23" s="155"/>
-      <c r="I23" s="155"/>
-      <c r="J23" s="155"/>
-      <c r="K23" s="155"/>
-      <c r="L23" s="155"/>
-      <c r="M23" s="155"/>
-      <c r="N23" s="155"/>
-      <c r="O23" s="155"/>
-      <c r="P23" s="156"/>
-      <c r="S23" s="86" t="s">
-        <v>54</v>
-      </c>
-      <c r="T23" s="87"/>
-      <c r="U23" s="42" t="s">
-        <v>56</v>
-      </c>
+    <row r="23" spans="2:19" s="2" customFormat="1" ht="14" thickBot="1">
+      <c r="B23" s="113"/>
+      <c r="C23" s="114"/>
+      <c r="D23" s="114"/>
+      <c r="E23" s="114"/>
+      <c r="F23" s="114"/>
+      <c r="G23" s="114"/>
+      <c r="H23" s="114"/>
+      <c r="I23" s="114"/>
+      <c r="J23" s="114"/>
+      <c r="K23" s="114"/>
+      <c r="L23" s="114"/>
+      <c r="M23" s="115"/>
+      <c r="N23" s="19"/>
+      <c r="O23" s="19"/>
+      <c r="Q23" s="39"/>
+      <c r="R23" s="118"/>
+      <c r="S23" s="119"/>
     </row>
-    <row r="24" spans="1:22" s="2" customFormat="1" ht="13.5" thickBot="1">
-      <c r="B24" s="157"/>
-      <c r="C24" s="158"/>
-      <c r="D24" s="158"/>
-      <c r="E24" s="158"/>
-      <c r="F24" s="158"/>
-      <c r="G24" s="158"/>
-      <c r="H24" s="158"/>
-      <c r="I24" s="158"/>
-      <c r="J24" s="158"/>
-      <c r="K24" s="158"/>
-      <c r="L24" s="158"/>
-      <c r="M24" s="158"/>
-      <c r="N24" s="158"/>
-      <c r="O24" s="158"/>
-      <c r="P24" s="159"/>
-      <c r="Q24" s="19"/>
-      <c r="R24" s="19"/>
-      <c r="T24" s="39"/>
-      <c r="U24" s="161"/>
-      <c r="V24" s="162"/>
+    <row r="24" spans="2:19" s="2" customFormat="1" ht="16" customHeight="1">
+      <c r="B24" s="4"/>
+      <c r="C24" s="4"/>
+      <c r="D24" s="4"/>
+      <c r="E24" s="4"/>
+      <c r="F24" s="24"/>
+      <c r="G24" s="24"/>
+      <c r="H24" s="24"/>
+      <c r="I24" s="24"/>
+      <c r="J24" s="4"/>
+      <c r="K24" s="103"/>
+      <c r="L24" s="18"/>
+      <c r="M24" s="18"/>
+      <c r="N24" s="18"/>
+      <c r="O24" s="18"/>
+      <c r="P24" s="4"/>
+      <c r="Q24" s="40"/>
+      <c r="R24" s="40"/>
+      <c r="S24" s="41"/>
     </row>
-    <row r="25" spans="1:22" s="2" customFormat="1" ht="15.95" customHeight="1">
-      <c r="B25" s="4"/>
+    <row r="25" spans="2:19" ht="14">
+      <c r="B25" s="19" t="s">
+        <v>2</v>
+      </c>
       <c r="C25" s="4"/>
       <c r="D25" s="4"/>
       <c r="E25" s="4"/>
@@ -2668,66 +2343,30 @@
       <c r="G25" s="24"/>
       <c r="H25" s="24"/>
       <c r="I25" s="24"/>
-      <c r="J25" s="24"/>
-      <c r="K25" s="24"/>
+      <c r="J25" s="4"/>
+      <c r="K25" s="104"/>
       <c r="L25" s="4"/>
-      <c r="M25" s="4"/>
-      <c r="N25" s="135"/>
-      <c r="O25" s="18"/>
-      <c r="P25" s="18"/>
-      <c r="Q25" s="18"/>
-      <c r="R25" s="18"/>
-      <c r="S25" s="4"/>
-      <c r="T25" s="40"/>
-      <c r="U25" s="40"/>
-      <c r="V25" s="41"/>
-    </row>
-    <row r="26" spans="1:22">
-      <c r="B26" s="19" t="s">
-        <v>2</v>
-      </c>
-      <c r="C26" s="4"/>
-      <c r="D26" s="4"/>
-      <c r="E26" s="4"/>
-      <c r="F26" s="24"/>
-      <c r="G26" s="24"/>
-      <c r="H26" s="24"/>
-      <c r="I26" s="24"/>
-      <c r="J26" s="24"/>
-      <c r="K26" s="24"/>
-      <c r="L26" s="4"/>
-      <c r="M26" s="4"/>
-      <c r="N26" s="136"/>
-      <c r="O26" s="4"/>
-      <c r="S26" s="85" t="s">
+      <c r="P25" s="82" t="s">
         <v>55</v>
       </c>
-      <c r="T26" s="42"/>
-      <c r="U26" s="160"/>
-      <c r="V26" s="160"/>
+      <c r="Q25" s="42"/>
+      <c r="R25" s="120"/>
+      <c r="S25" s="120"/>
     </row>
   </sheetData>
   <dataConsolidate/>
-  <mergeCells count="19">
-    <mergeCell ref="S9:V9"/>
-    <mergeCell ref="S10:V10"/>
-    <mergeCell ref="S11:V11"/>
-    <mergeCell ref="S12:V12"/>
-    <mergeCell ref="L18:M18"/>
-    <mergeCell ref="L17:M17"/>
-    <mergeCell ref="S2:T2"/>
-    <mergeCell ref="S3:T3"/>
-    <mergeCell ref="S4:V5"/>
-    <mergeCell ref="S6:V7"/>
-    <mergeCell ref="U2:V2"/>
-    <mergeCell ref="U3:V3"/>
-    <mergeCell ref="L14:M14"/>
-    <mergeCell ref="L15:M16"/>
-    <mergeCell ref="N15:N16"/>
-    <mergeCell ref="B22:P24"/>
-    <mergeCell ref="U26:V26"/>
-    <mergeCell ref="U24:V24"/>
-    <mergeCell ref="U20:V20"/>
+  <mergeCells count="11">
+    <mergeCell ref="K15:K16"/>
+    <mergeCell ref="P9:S9"/>
+    <mergeCell ref="P10:S10"/>
+    <mergeCell ref="P11:S11"/>
+    <mergeCell ref="P12:S12"/>
+    <mergeCell ref="P2:Q2"/>
+    <mergeCell ref="P3:Q3"/>
+    <mergeCell ref="P4:S5"/>
+    <mergeCell ref="P6:S7"/>
+    <mergeCell ref="R2:S2"/>
+    <mergeCell ref="R3:S3"/>
   </mergeCells>
   <phoneticPr fontId="12" type="noConversion"/>
   <printOptions horizontalCentered="1"/>
@@ -2741,12 +2380,12 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13"/>
   <sheetData/>
   <phoneticPr fontId="12" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -2758,12 +2397,12 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13"/>
   <sheetData/>
   <phoneticPr fontId="12" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
modify the orderline entry table
</commit_message>
<xml_diff>
--- a/backend/static/PO TemplateLT.xlsx
+++ b/backend/static/PO TemplateLT.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dongxiaomu/Desktop/iMIS/backend/static/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA4D89D4-A759-C549-B4E4-FA4F779837BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C817A02-6B5D-C545-B367-CE86D496D3AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -343,9 +343,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="4">
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
-    <numFmt numFmtId="166" formatCode="dd\-mmm\-yy"/>
-    <numFmt numFmtId="167" formatCode="[$-409]d\-mmm\-yy;@"/>
-    <numFmt numFmtId="168" formatCode="&quot;$&quot;#,##0.0000"/>
+    <numFmt numFmtId="165" formatCode="dd\-mmm\-yy"/>
+    <numFmt numFmtId="166" formatCode="[$-409]d\-mmm\-yy;@"/>
+    <numFmt numFmtId="167" formatCode="&quot;$&quot;#,##0.0000"/>
   </numFmts>
   <fonts count="25">
     <font>
@@ -918,7 +918,7 @@
     <xf numFmtId="49" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -983,7 +983,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="168" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1027,7 +1027,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="168" fontId="5" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="5" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1174,13 +1174,37 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="167" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="167" fontId="9" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="9" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment shrinkToFit="1"/>
+    </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
@@ -1195,30 +1219,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment shrinkToFit="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1724,7 +1724,7 @@
   <dimension ref="B1:S25"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="80" workbookViewId="0">
-      <selection activeCell="H30" sqref="H30"/>
+      <selection activeCell="R19" sqref="R19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="13"/>
@@ -1790,12 +1790,12 @@
       <c r="M2" s="4"/>
       <c r="N2" s="5"/>
       <c r="O2" s="5"/>
-      <c r="P2" s="121" t="s">
+      <c r="P2" s="129" t="s">
         <v>38</v>
       </c>
-      <c r="Q2" s="121"/>
-      <c r="R2" s="124"/>
-      <c r="S2" s="125"/>
+      <c r="Q2" s="129"/>
+      <c r="R2" s="132"/>
+      <c r="S2" s="133"/>
     </row>
     <row r="3" spans="2:19" s="2" customFormat="1" ht="16" customHeight="1">
       <c r="B3" s="19" t="s">
@@ -1814,12 +1814,12 @@
       <c r="M3" s="1"/>
       <c r="N3" s="6"/>
       <c r="O3" s="6"/>
-      <c r="P3" s="121" t="s">
+      <c r="P3" s="129" t="s">
         <v>37</v>
       </c>
-      <c r="Q3" s="121"/>
-      <c r="R3" s="124"/>
-      <c r="S3" s="125"/>
+      <c r="Q3" s="129"/>
+      <c r="R3" s="132"/>
+      <c r="S3" s="133"/>
     </row>
     <row r="4" spans="2:19" s="2" customFormat="1" ht="12.75" customHeight="1">
       <c r="B4" s="19" t="s">
@@ -1838,12 +1838,12 @@
       <c r="M4" s="1"/>
       <c r="N4" s="1"/>
       <c r="O4" s="1"/>
-      <c r="P4" s="122" t="s">
+      <c r="P4" s="130" t="s">
         <v>46</v>
       </c>
-      <c r="Q4" s="122"/>
-      <c r="R4" s="122"/>
-      <c r="S4" s="122"/>
+      <c r="Q4" s="130"/>
+      <c r="R4" s="130"/>
+      <c r="S4" s="130"/>
     </row>
     <row r="5" spans="2:19" s="2" customFormat="1">
       <c r="B5" s="4"/>
@@ -1860,10 +1860,10 @@
       <c r="M5" s="1"/>
       <c r="N5" s="1"/>
       <c r="O5" s="1"/>
-      <c r="P5" s="122"/>
-      <c r="Q5" s="122"/>
-      <c r="R5" s="122"/>
-      <c r="S5" s="122"/>
+      <c r="P5" s="130"/>
+      <c r="Q5" s="130"/>
+      <c r="R5" s="130"/>
+      <c r="S5" s="130"/>
     </row>
     <row r="6" spans="2:19" s="2" customFormat="1" ht="12.75" customHeight="1">
       <c r="B6" s="19"/>
@@ -1880,12 +1880,12 @@
       <c r="M6" s="1"/>
       <c r="N6" s="1"/>
       <c r="O6" s="1"/>
-      <c r="P6" s="123" t="s">
+      <c r="P6" s="131" t="s">
         <v>20</v>
       </c>
-      <c r="Q6" s="123"/>
-      <c r="R6" s="123"/>
-      <c r="S6" s="123"/>
+      <c r="Q6" s="131"/>
+      <c r="R6" s="131"/>
+      <c r="S6" s="131"/>
     </row>
     <row r="7" spans="2:19" s="2" customFormat="1" ht="18" customHeight="1" thickBot="1">
       <c r="B7" s="4"/>
@@ -1902,10 +1902,10 @@
       <c r="M7" s="1"/>
       <c r="N7" s="1"/>
       <c r="O7" s="1"/>
-      <c r="P7" s="123"/>
-      <c r="Q7" s="123"/>
-      <c r="R7" s="123"/>
-      <c r="S7" s="123"/>
+      <c r="P7" s="131"/>
+      <c r="Q7" s="131"/>
+      <c r="R7" s="131"/>
+      <c r="S7" s="131"/>
     </row>
     <row r="8" spans="2:19" s="22" customFormat="1" ht="16" customHeight="1">
       <c r="B8" s="67" t="s">
@@ -1950,10 +1950,10 @@
       <c r="M9" s="47"/>
       <c r="N9" s="47"/>
       <c r="O9" s="48"/>
-      <c r="P9" s="128"/>
-      <c r="Q9" s="129"/>
-      <c r="R9" s="129"/>
-      <c r="S9" s="130"/>
+      <c r="P9" s="123"/>
+      <c r="Q9" s="124"/>
+      <c r="R9" s="124"/>
+      <c r="S9" s="125"/>
     </row>
     <row r="10" spans="2:19" s="25" customFormat="1" ht="16">
       <c r="B10" s="54"/>
@@ -1972,10 +1972,10 @@
       <c r="M10"/>
       <c r="N10"/>
       <c r="O10" s="50"/>
-      <c r="P10" s="128"/>
-      <c r="Q10" s="129"/>
-      <c r="R10" s="129"/>
-      <c r="S10" s="130"/>
+      <c r="P10" s="123"/>
+      <c r="Q10" s="124"/>
+      <c r="R10" s="124"/>
+      <c r="S10" s="125"/>
     </row>
     <row r="11" spans="2:19" s="25" customFormat="1" ht="16">
       <c r="B11" s="54"/>
@@ -1994,10 +1994,10 @@
       <c r="M11"/>
       <c r="N11"/>
       <c r="O11" s="50"/>
-      <c r="P11" s="128"/>
-      <c r="Q11" s="129"/>
-      <c r="R11" s="129"/>
-      <c r="S11" s="130"/>
+      <c r="P11" s="123"/>
+      <c r="Q11" s="124"/>
+      <c r="R11" s="124"/>
+      <c r="S11" s="125"/>
     </row>
     <row r="12" spans="2:19" s="25" customFormat="1" ht="17" thickBot="1">
       <c r="B12" s="56"/>
@@ -2016,10 +2016,10 @@
       <c r="M12" s="52"/>
       <c r="N12" s="52"/>
       <c r="O12" s="53"/>
-      <c r="P12" s="131"/>
-      <c r="Q12" s="132"/>
-      <c r="R12" s="132"/>
-      <c r="S12" s="133"/>
+      <c r="P12" s="126"/>
+      <c r="Q12" s="127"/>
+      <c r="R12" s="127"/>
+      <c r="S12" s="128"/>
     </row>
     <row r="13" spans="2:19" ht="7" customHeight="1" thickBot="1">
       <c r="C13" s="26"/>
@@ -2108,7 +2108,7 @@
       <c r="J15" s="80" t="s">
         <v>40</v>
       </c>
-      <c r="K15" s="126" t="s">
+      <c r="K15" s="121" t="s">
         <v>41</v>
       </c>
       <c r="L15" s="64" t="s">
@@ -2154,7 +2154,7 @@
         <v>45</v>
       </c>
       <c r="J16" s="81"/>
-      <c r="K16" s="127"/>
+      <c r="K16" s="122"/>
       <c r="L16" s="27" t="s">
         <v>12</v>
       </c>
@@ -2230,10 +2230,7 @@
       <c r="Q19" s="36" t="s">
         <v>42</v>
       </c>
-      <c r="R19" s="116" t="e">
-        <f>SUM(#REF!)</f>
-        <v>#REF!</v>
-      </c>
+      <c r="R19" s="116"/>
       <c r="S19" s="117"/>
     </row>
     <row r="20" spans="2:19" ht="16" customHeight="1" thickTop="1">
@@ -2356,17 +2353,17 @@
   </sheetData>
   <dataConsolidate/>
   <mergeCells count="11">
-    <mergeCell ref="K15:K16"/>
-    <mergeCell ref="P9:S9"/>
-    <mergeCell ref="P10:S10"/>
-    <mergeCell ref="P11:S11"/>
-    <mergeCell ref="P12:S12"/>
     <mergeCell ref="P2:Q2"/>
     <mergeCell ref="P3:Q3"/>
     <mergeCell ref="P4:S5"/>
     <mergeCell ref="P6:S7"/>
     <mergeCell ref="R2:S2"/>
     <mergeCell ref="R3:S3"/>
+    <mergeCell ref="K15:K16"/>
+    <mergeCell ref="P9:S9"/>
+    <mergeCell ref="P10:S10"/>
+    <mergeCell ref="P11:S11"/>
+    <mergeCell ref="P12:S12"/>
   </mergeCells>
   <phoneticPr fontId="12" type="noConversion"/>
   <printOptions horizontalCentered="1"/>

</xml_diff>